<commit_message>
feat: começando feature engineering
</commit_message>
<xml_diff>
--- a/dic_auxiliar.xlsx
+++ b/dic_auxiliar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\AQUI PRA CLONAR\case_datarisk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20A8CE43-ACF5-429E-99F9-D2844079384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A976D1CD-74BE-493F-AA70-C2EB560848C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D92C70BA-F811-437E-A52B-1CE4CE977F7C}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>id_cliente</t>
   </si>
   <si>
-    <t>Identificador Ãºnico do cliente</t>
-  </si>
-  <si>
     <t>sexo</t>
   </si>
   <si>
@@ -64,9 +61,6 @@
     <t>qtd_membros_familia</t>
   </si>
   <si>
-    <t>Quantidade total de membros da famÃ­lia</t>
-  </si>
-  <si>
     <t>renda_anual</t>
   </si>
   <si>
@@ -76,15 +70,9 @@
     <t>tipo_renda</t>
   </si>
   <si>
-    <t>Tipo de fonte de renda (trabalho, pensÃ£o, aposentadoria, etc.)</t>
-  </si>
-  <si>
     <t>ocupacao</t>
   </si>
   <si>
-    <t>OcupaÃ§Ã£o profissional do cliente</t>
-  </si>
-  <si>
     <t>tipo_organizacao</t>
   </si>
   <si>
@@ -94,9 +82,6 @@
     <t>nivel_educacao</t>
   </si>
   <si>
-    <t>NÃ­vel de escolaridade alcanÃ§ado</t>
-  </si>
-  <si>
     <t>estado_civil</t>
   </si>
   <si>
@@ -106,9 +91,6 @@
     <t>tipo_moradia</t>
   </si>
   <si>
-    <t>Tipo de moradia (casa prÃ³pria, alugada, com parentes, etc.)</t>
-  </si>
-  <si>
     <t>possui_carro</t>
   </si>
   <si>
@@ -118,21 +100,12 @@
     <t>possui_imovel</t>
   </si>
   <si>
-    <t>Indicador se o cliente possui imÃ³vel (Y/N)</t>
-  </si>
-  <si>
     <t>nota_regiao_cliente</t>
   </si>
   <si>
-    <t>AvaliaÃ§Ã£o de risco da regiÃ£o de residÃªncia do cliente</t>
-  </si>
-  <si>
     <t>nota_regiao_cliente_cidade</t>
   </si>
   <si>
-    <t>AvaliaÃ§Ã£o de risco da regiÃ£o, ajustada para a cidade</t>
-  </si>
-  <si>
     <t>base_submissao</t>
   </si>
   <si>
@@ -151,48 +124,27 @@
     <t>hora_solicitacao</t>
   </si>
   <si>
-    <t>Hora do dia em que a solicitaÃ§Ã£o foi realizada</t>
-  </si>
-  <si>
     <t>tipo_contrato</t>
   </si>
   <si>
-    <t>Tipo de contrato solicitado (ex: crÃ©dito pessoal, rotativo, etc.)</t>
-  </si>
-  <si>
     <t>valor_credito</t>
   </si>
   <si>
-    <t>Valor total do crÃ©dito solicitado</t>
-  </si>
-  <si>
     <t>valor_bem</t>
   </si>
   <si>
-    <t>Valor do bem financiado, quando aplicÃ¡vel</t>
-  </si>
-  <si>
     <t>valor_parcela</t>
   </si>
   <si>
-    <t>Valor da parcela periÃ³dica estimada para pagamento do emprÃ©stimo</t>
-  </si>
-  <si>
     <t>historico_emprestimos</t>
   </si>
   <si>
     <t>id_contrato</t>
   </si>
   <si>
-    <t>Identificador Ãºnico do contrato de emprÃ©stimo</t>
-  </si>
-  <si>
     <t>Identificador do cliente associado ao contrato</t>
   </si>
   <si>
-    <t>Tipo de contrato (crÃ©dito pessoal, rotativo, etc.)</t>
-  </si>
-  <si>
     <t>status_contrato</t>
   </si>
   <si>
@@ -208,9 +160,6 @@
     <t>data_liberacao</t>
   </si>
   <si>
-    <t>Data em que o crÃ©dito foi liberado</t>
-  </si>
-  <si>
     <t>data_primeiro_vencimento</t>
   </si>
   <si>
@@ -220,21 +169,12 @@
     <t>data_ultimo_vencimento_original</t>
   </si>
   <si>
-    <t>Data original prevista para a Ãºltima parcela</t>
-  </si>
-  <si>
     <t>data_ultimo_vencimento</t>
   </si>
   <si>
-    <t>Data final revisada da Ãºltima parcela</t>
-  </si>
-  <si>
     <t>data_encerramento</t>
   </si>
   <si>
-    <t>Data em que o contrato foi encerrado (por quitaÃ§Ã£o, cancelamento, etc.)</t>
-  </si>
-  <si>
     <t>valor_solicitado</t>
   </si>
   <si>
@@ -244,12 +184,6 @@
     <t>Valor efetivamente liberado</t>
   </si>
   <si>
-    <t>Valor do bem adquirido, quando aplicÃ¡vel</t>
-  </si>
-  <si>
-    <t>Valor estimado da parcela periÃ³dica</t>
-  </si>
-  <si>
     <t>valor_entrada</t>
   </si>
   <si>
@@ -271,15 +205,9 @@
     <t>taxa_juros_padrao</t>
   </si>
   <si>
-    <t>Taxa de juros padrÃ£o aplicada</t>
-  </si>
-  <si>
     <t>taxa_juros_promocional</t>
   </si>
   <si>
-    <t>Taxa promocional (se aplicÃ¡vel)</t>
-  </si>
-  <si>
     <t>tipo_pagamento</t>
   </si>
   <si>
@@ -289,9 +217,6 @@
     <t>finalidade_emprestimo</t>
   </si>
   <si>
-    <t>Finalidade declarada para o uso do emprÃ©stimo</t>
-  </si>
-  <si>
     <t>tipo_cliente</t>
   </si>
   <si>
@@ -307,9 +232,6 @@
     <t>tipo_portfolio</t>
   </si>
   <si>
-    <t>Tipo de portfÃ³lio (interno, externo, etc.)</t>
-  </si>
-  <si>
     <t>tipo_produto</t>
   </si>
   <si>
@@ -325,9 +247,6 @@
     <t>combinacao_produto</t>
   </si>
   <si>
-    <t>CombinaÃ§Ã£o de produtos oferecida</t>
-  </si>
-  <si>
     <t>setor_vendedor</t>
   </si>
   <si>
@@ -337,33 +256,15 @@
     <t>canal_venda</t>
   </si>
   <si>
-    <t>Canal utilizado para originaÃ§Ã£o da venda</t>
-  </si>
-  <si>
     <t>area_venda</t>
   </si>
   <si>
-    <t>Ãrea ou localizaÃ§Ã£o da venda</t>
-  </si>
-  <si>
-    <t>Dia da semana em que a solicitaÃ§Ã£o foi iniciada</t>
-  </si>
-  <si>
-    <t>Hora do dia em que a solicitaÃ§Ã£o foi iniciada</t>
-  </si>
-  <si>
     <t>flag_ultima_solicitacao_contrato</t>
   </si>
   <si>
-    <t>Indica se foi a Ãºltima solicitaÃ§Ã£o para aquele contrato</t>
-  </si>
-  <si>
     <t>flag_ultima_solicitacao_dia</t>
   </si>
   <si>
-    <t>Indica se foi a Ãºltima solicitaÃ§Ã£o feita no mesmo dia</t>
-  </si>
-  <si>
     <t>motivo_recusa</t>
   </si>
   <si>
@@ -373,36 +274,21 @@
     <t>acompanhantes_cliente</t>
   </si>
   <si>
-    <t>Tipo de acompanhantes no momento da solicitaÃ§Ã£o (ex: sozinho, famÃ­lia)</t>
-  </si>
-  <si>
     <t>flag_seguro_contratado</t>
   </si>
   <si>
-    <t>Indica se o cliente contratou seguro junto com o crÃ©dito</t>
-  </si>
-  <si>
     <t>historico_parcelas</t>
   </si>
   <si>
-    <t>Identificador do contrato de emprÃ©stimo</t>
-  </si>
-  <si>
     <t>Identificador do cliente</t>
   </si>
   <si>
     <t>versao_parcela</t>
   </si>
   <si>
-    <t>VersÃ£o da parcela dentro do contrato (caso haja alteraÃ§Ãµes)</t>
-  </si>
-  <si>
     <t>numero_parcela</t>
   </si>
   <si>
-    <t>NÃºmero sequencial da parcela dentro do contrato</t>
-  </si>
-  <si>
     <t>data_prevista_pagamento</t>
   </si>
   <si>
@@ -425,6 +311,120 @@
   </si>
   <si>
     <t>Valor efetivamente pago pelo cliente</t>
+  </si>
+  <si>
+    <t>Identificador único do cliente</t>
+  </si>
+  <si>
+    <t>Quantidade total de membros da família</t>
+  </si>
+  <si>
+    <t>Tipo de fonte de renda (trabalho, pensão, aposentadoria, etc.)</t>
+  </si>
+  <si>
+    <t>Ocupação profissional do cliente</t>
+  </si>
+  <si>
+    <t>Nível de escolaridade alcançado</t>
+  </si>
+  <si>
+    <t>Tipo de moradia (casa própria, alugada, com parentes, etc.)</t>
+  </si>
+  <si>
+    <t>Indicador se o cliente possui imóvel (Y/N)</t>
+  </si>
+  <si>
+    <t>Avaliação de risco da região de residência do cliente</t>
+  </si>
+  <si>
+    <t>Avaliação de risco da região, ajustada para a cidade</t>
+  </si>
+  <si>
+    <t>Hora do dia em que a solicitação foi realizada</t>
+  </si>
+  <si>
+    <t>Tipo de contrato solicitado (ex: crédito pessoal, rotativo, etc.)</t>
+  </si>
+  <si>
+    <t>Valor total do crédito solicitado</t>
+  </si>
+  <si>
+    <t>Valor do bem financiado, quando aplicável</t>
+  </si>
+  <si>
+    <t>Valor da parcela periódica estimada para pagamento do empréstimo</t>
+  </si>
+  <si>
+    <t>Identificador único do contrato de empréstimo</t>
+  </si>
+  <si>
+    <t>Tipo de contrato (crédito pessoal, rotativo, etc.)</t>
+  </si>
+  <si>
+    <t>Data em que o crédito foi liberado</t>
+  </si>
+  <si>
+    <t>Data original prevista para a última parcela</t>
+  </si>
+  <si>
+    <t>Data final revisada da última parcela</t>
+  </si>
+  <si>
+    <t>Data em que o contrato foi encerrado (por quitação, cancelamento, etc.)</t>
+  </si>
+  <si>
+    <t>Valor do bem adquirido, quando aplicável</t>
+  </si>
+  <si>
+    <t>Valor estimado da parcela periódica</t>
+  </si>
+  <si>
+    <t>Taxa de juros padrão aplicada</t>
+  </si>
+  <si>
+    <t>Taxa promocional (se aplicável)</t>
+  </si>
+  <si>
+    <t>Finalidade declarada para o uso do empréstimo</t>
+  </si>
+  <si>
+    <t>Tipo de portfólio (interno, externo, etc.)</t>
+  </si>
+  <si>
+    <t>Combinação de produtos oferecida</t>
+  </si>
+  <si>
+    <t>Canal utilizado para originação da venda</t>
+  </si>
+  <si>
+    <t>Área ou localização da venda</t>
+  </si>
+  <si>
+    <t>Dia da semana em que a solicitação foi iniciada</t>
+  </si>
+  <si>
+    <t>Hora do dia em que a solicitação foi iniciada</t>
+  </si>
+  <si>
+    <t>Indica se foi a última solicitação para aquele contrato</t>
+  </si>
+  <si>
+    <t>Indica se foi a última solicitação feita no mesmo dia</t>
+  </si>
+  <si>
+    <t>Tipo de acompanhantes no momento da solicitação (ex: sozinho, família)</t>
+  </si>
+  <si>
+    <t>Indica se o cliente contratou seguro junto com o crédito</t>
+  </si>
+  <si>
+    <t>Identificador do contrato de empréstimo</t>
+  </si>
+  <si>
+    <t>Versão da parcela dentro do contrato (caso haja alterações)</t>
+  </si>
+  <si>
+    <t>Número sequencial da parcela dentro do contrato</t>
   </si>
 </sst>
 </file>
@@ -908,8 +908,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1287,7 +1288,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4068E4C-371B-44FF-947B-94338A5AD4F9}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1296,14 +1299,14 @@
     <col min="3" max="3" width="71.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1315,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,10 +1326,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,10 +1337,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,10 +1348,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,10 +1359,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1367,10 +1370,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1378,10 +1381,10 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1389,10 +1392,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1400,10 +1403,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1411,10 +1414,10 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1422,10 +1425,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1433,10 +1436,10 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1444,10 +1447,10 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1455,10 +1458,10 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1466,10 +1469,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1477,597 +1480,598 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
         <v>51</v>
-      </c>
-      <c r="B36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C44" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
-        <v>88</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B47" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B49" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C49" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C56" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="C59" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B61" t="s">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
         <v>4</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B67" t="s">
-        <v>126</v>
+        <v>88</v>
       </c>
       <c r="C67" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C69" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="C70" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{E4068E4C-371B-44FF-947B-94338A5AD4F9}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>